<commit_message>
[1] Latest head banging on Excel chart format.
</commit_message>
<xml_diff>
--- a/Codex/dat/unittest-time-all.xlsx
+++ b/Codex/dat/unittest-time-all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsloan/src/com-diag-codex/Codex/dat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D6DB073E-B532-8E4D-9537-38C3C1553EDB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C3D03AE8-D489-EF4F-8E9A-2E3763C0C828}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20300" yWindow="3060" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{58600780-870C-514C-A633-550479BCFCCC}"/>
+    <workbookView xWindow="14180" yWindow="8120" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{58600780-870C-514C-A633-550479BCFCCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,69 +19,6 @@
     <sheet name="Chart2" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1:$U$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$U$2</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$A$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$A$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$A$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$A$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$A$1:$U$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$U$2</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$A$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$A$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$A$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$A$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$A$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$A$1:$U$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$A$2:$U$2</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$A$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$A$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$A$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$A$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$A$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$A$1:$U$1</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$A$2:$U$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$A$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$A$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$A$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$A$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$A$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$A$1:$U$1</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$A$2:$U$2</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$A$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$A$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$A$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$A$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$A$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$A$1:$U$1</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$A$2:$U$2</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$A$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$A$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$A$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$A$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$A$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Sheet2!$A$1:$U$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Sheet2!$A$2:$U$2</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Sheet2!$A$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Sheet2!$A$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Sheet2!$A$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Sheet2!$A$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Sheet2!$A$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Sheet2!$A$1:$U$1</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Sheet2!$A$2:$U$2</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Sheet2!$A$3:$U$3</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Sheet2!$A$4:$U$4</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Sheet2!$A$5:$U$5</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Sheet2!$A$6:$U$6</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Sheet2!$A$7:$U$7</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$1:$U$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$2:$U$2</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$3:$U$3</definedName>
     <definedName name="unittest_time_control_matrix" localSheetId="0">Sheet1!$A$1:$U$7</definedName>
     <definedName name="unittest_time_core_matrix" localSheetId="2">Sheet2!$A$1:$U$7</definedName>
   </definedNames>
@@ -224,11 +161,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -299,14 +236,122 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>64</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$A$1:$U$1</c:f>
@@ -388,14 +433,122 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>128</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$A$2:$U$2</c:f>
@@ -477,14 +630,122 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>256</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent3">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$A$3:$U$3</c:f>
@@ -566,14 +827,122 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:v>512</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$A$4:$U$4</c:f>
@@ -655,14 +1024,122 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:v>1024</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent5">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$A$5:$U$5</c:f>
@@ -744,14 +1221,122 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
+          <c:tx>
+            <c:v>2048</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent6">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$A$6:$U$6</c:f>
@@ -833,16 +1418,127 @@
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
+          <c:tx>
+            <c:v>4096</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$A$7:$U$7</c:f>
@@ -925,187 +1621,766 @@
           <c:bandFmt>
             <c:idx val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent1">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="1"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="2"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent3">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="3"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="4"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent5">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent6">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="7"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="8"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="9"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="10"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="11"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="12"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="13"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="14"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
@@ -1120,6 +2395,42 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>TOTAL CPU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1144,8 +2455,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1184,6 +2495,41 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>DATA</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1203,8 +2549,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1226,13 +2572,54 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>BUFFER</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1244,8 +2631,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1285,8 +2672,8 @@
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1357,13 +2744,27 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1371,9 +2772,42 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>unittest-time-core-matrix</a:t>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>unittest-time-core-matrix </a:t>
             </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1433,14 +2867,122 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>64</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$A$1:$U$1</c:f>
@@ -1522,14 +3064,122 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>128</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent2">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$A$2:$U$2</c:f>
@@ -1611,14 +3261,122 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>256</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent3">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$A$3:$U$3</c:f>
@@ -1700,14 +3458,122 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:v>512</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent4">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$A$4:$U$4</c:f>
@@ -1789,14 +3655,122 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:v>1024</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent5">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$A$5:$U$5</c:f>
@@ -1878,14 +3852,122 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
+          <c:tx>
+            <c:v>2048</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent6">
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$A$6:$U$6</c:f>
@@ -1967,16 +4049,127 @@
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
+          <c:tx>
+            <c:v>4096</c:v>
+          </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln/>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="110000"/>
+                    <a:satMod val="105000"/>
+                    <a:tint val="67000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="103000"/>
+                    <a:tint val="73000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumMod val="105000"/>
+                    <a:satMod val="109000"/>
+                    <a:tint val="81000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
             <a:effectLst/>
-            <a:sp3d/>
+            <a:sp3d contourW="9525">
+              <a:contourClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:shade val="95000"/>
+                </a:schemeClr>
+              </a:contourClr>
+            </a:sp3d>
           </c:spPr>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="21"/>
+              <c:pt idx="0">
+                <c:v>4096</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>8192</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>16384</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>32768</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>65536</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>131072</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>262144</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>524288</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>1048576</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>2097152</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>4194304</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>8388608</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>16777216</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>33554432</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>67108864</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>134217728</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>268435456</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>536870912</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>1073741824</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>2147483648</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>4294967296</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet2!$A$7:$U$7</c:f>
@@ -2059,187 +4252,766 @@
           <c:bandFmt>
             <c:idx val="0"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent1">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="1"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="2"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent3">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="3"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="4"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent5">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent6">
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="7"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="8"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="9"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="10"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="11"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="12"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="13"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
           <c:bandFmt>
             <c:idx val="14"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln/>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="110000"/>
+                      <a:satMod val="105000"/>
+                      <a:tint val="67000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="103000"/>
+                      <a:tint val="73000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="80000"/>
+                      <a:lumOff val="20000"/>
+                      <a:lumMod val="105000"/>
+                      <a:satMod val="109000"/>
+                      <a:tint val="81000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
               <a:effectLst/>
-              <a:sp3d/>
+              <a:sp3d contourW="9525">
+                <a:contourClr>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                    <a:shade val="95000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
           </c:bandFmt>
         </c:bandFmts>
@@ -2254,6 +5026,42 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>TOTAL CPU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2278,8 +5086,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2318,6 +5126,41 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>DATA</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2337,8 +5180,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2360,13 +5203,54 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>BUFFER</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2378,8 +5262,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2419,8 +5303,8 @@
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -2475,7 +5359,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BB0CC125-4BFF-384A-9113-A4F4AF1AB68E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="134" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="133" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2486,7 +5370,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F7E5C3D7-DF68-8241-AA70-142EC64FF7A0}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="134" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2497,7 +5381,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8681493" cy="6293134"/>
+    <xdr:ext cx="8675077" cy="6291385"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2530,7 +5414,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8673411" cy="6290930"/>
+    <xdr:ext cx="8681493" cy="6293134"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3341,7 +6225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C7CF39-CD22-894D-A5DE-643CB554D023}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>